<commit_message>
LineSeparator ant option is implemented.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoAntTaskTask.xlsx
+++ b/meta/program/BlancoAntTaskTask.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoAntTask/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8626CA3B-C18B-274E-AD19-CB33ADC4BC4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557A6156-77EB-7C45-A77F-CDFCCC5D391F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="860"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anttask" sheetId="1" r:id="rId1"/>
@@ -28,19 +28,11 @@
     <definedName name="必須">config!$C$5:$C$6</definedName>
   </definedNames>
   <calcPr calcId="92512"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -188,12 +180,33 @@
     <t>自動生成するソースファイルの文字エンコーディングを指定します。</t>
     <phoneticPr fontId="5"/>
   </si>
+  <si>
+    <t>lineSeparator</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>LF</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>自動生成するソースコードの改行コードを、LF, CR, CRLFで指定します。</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ジドウセイセイ </t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">カイギョウコード </t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -232,6 +245,12 @@
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -614,7 +633,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -706,6 +725,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -714,22 +745,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1129,13 +1154,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -1177,10 +1204,10 @@
       <c r="F5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="52"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
@@ -1189,10 +1216,10 @@
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="52"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
@@ -1201,10 +1228,10 @@
       <c r="F7"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="52" t="s">
+      <c r="A8" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="52"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="6" t="s">
         <v>26</v>
       </c>
@@ -1214,10 +1241,10 @@
       <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="52"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1245,34 +1272,34 @@
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="53" t="s">
+      <c r="E12" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="54" t="s">
+      <c r="F12" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="55"/>
+      <c r="G12" s="50"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="47"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="55"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="50"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="41">
@@ -1307,10 +1334,10 @@
       <c r="E15" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="50" t="s">
+      <c r="F15" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="51"/>
+      <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" ht="27.5" customHeight="1">
       <c r="A16" s="42">
@@ -1326,10 +1353,10 @@
       <c r="E16" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="51"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" ht="27" customHeight="1">
       <c r="A17" s="42">
@@ -1343,18 +1370,28 @@
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="34"/>
-      <c r="F17" s="50" t="s">
+      <c r="F17" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="51"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="42"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
+      <c r="A18" s="42">
+        <v>5</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>17</v>
+      </c>
       <c r="D18" s="45"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
+      <c r="E18" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="57" t="s">
+        <v>40</v>
+      </c>
       <c r="G18" s="36"/>
     </row>
     <row r="19" spans="1:7">
@@ -1431,12 +1468,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
@@ -1444,17 +1475,23 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F42">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F42" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D26">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D26" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C26">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C14:C26" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>型リスト</formula1>
     </dataValidation>
   </dataValidations>
@@ -1467,7 +1504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>